<commit_message>
Some updates to Fold.
</commit_message>
<xml_diff>
--- a/data/deeltijdswerk.xlsx
+++ b/data/deeltijdswerk.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\E8\0557-LFS\Docs\website\2020 (data 2020)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gustv\Projects\synthasizer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EE9D06-5977-46AB-897D-06291A047808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB55625-3560-4817-8446-AA27B7A96FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4500" yWindow="3860" windowWidth="28800" windowHeight="15370" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regime" sheetId="4" r:id="rId1"/>
     <sheet name="Sector" sheetId="1" r:id="rId2"/>
     <sheet name="Reden" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="48">
   <si>
     <t>Totaal</t>
   </si>
@@ -275,7 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -341,6 +343,7 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -380,9 +383,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Standaard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -399,7 +412,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -721,28 +734,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.109375" style="4" customWidth="1"/>
-    <col min="2" max="8" width="9.109375" style="4"/>
+    <col min="1" max="1" width="27.08984375" style="4" customWidth="1"/>
+    <col min="2" max="8" width="9.08984375" style="4"/>
     <col min="9" max="9" width="10" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="4"/>
+    <col min="10" max="16384" width="9.08984375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="17"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" s="16">
         <v>2017</v>
       </c>
@@ -758,7 +771,7 @@
       <c r="M3" s="34"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -772,7 +785,7 @@
       <c r="M4" s="4"/>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>36</v>
       </c>
@@ -792,7 +805,7 @@
       <c r="M5" s="34"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>40</v>
       </c>
@@ -812,7 +825,7 @@
       <c r="M6" s="34"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
@@ -832,7 +845,7 @@
       <c r="M7" s="34"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>42</v>
       </c>
@@ -852,7 +865,7 @@
       <c r="M8" s="34"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -864,7 +877,7 @@
       <c r="M9" s="35"/>
       <c r="N9" s="6"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>36</v>
       </c>
@@ -884,7 +897,7 @@
       <c r="M10" s="35"/>
       <c r="N10" s="6"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>40</v>
       </c>
@@ -904,7 +917,7 @@
       <c r="M11" s="35"/>
       <c r="N11" s="6"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>41</v>
       </c>
@@ -924,7 +937,7 @@
       <c r="M12" s="34"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>42</v>
       </c>
@@ -944,7 +957,7 @@
       <c r="M13" s="34"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>23</v>
       </c>
@@ -956,7 +969,7 @@
       <c r="M14" s="34"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>36</v>
       </c>
@@ -976,7 +989,7 @@
       <c r="M15" s="34"/>
       <c r="N15" s="1"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>40</v>
       </c>
@@ -995,7 +1008,7 @@
       <c r="F16" s="14"/>
       <c r="M16" s="34"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>41</v>
       </c>
@@ -1014,7 +1027,7 @@
       <c r="F17" s="14"/>
       <c r="M17" s="34"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>42</v>
       </c>
@@ -1032,102 +1045,102 @@
       </c>
       <c r="F18" s="14"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D19" s="13"/>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="41" t="s">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="41"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="41"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="41"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="42"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-    </row>
-    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="41" t="s">
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" s="42"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="42"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="42"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" s="43"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+    </row>
+    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="41"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="41"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" s="42"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" s="42"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1149,74 +1162,74 @@
       <selection activeCell="K3" sqref="K3:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="79" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="8.88671875" style="4"/>
-    <col min="17" max="17" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="24" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="9.109375" style="4"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="8.90625" style="4"/>
+    <col min="17" max="17" width="10.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="24" width="10.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="9.08984375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17"/>
     </row>
-    <row r="3" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="43">
+    <row r="3" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="44">
         <v>2017</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="43">
+      <c r="C3" s="45"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="44">
         <v>2018</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="43">
+      <c r="F3" s="45"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="44">
         <v>2019</v>
       </c>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="43">
+      <c r="I3" s="45"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="44">
         <v>2020</v>
       </c>
-      <c r="L3" s="44"/>
-      <c r="M3" s="45"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="L3" s="45"/>
+      <c r="M3" s="46"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="43" t="s">
+      <c r="C4" s="45"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="44"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="43" t="s">
+      <c r="F4" s="45"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="44"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="43" t="s">
+      <c r="I4" s="45"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="L4" s="44"/>
-      <c r="M4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="46"/>
       <c r="N4" s="4"/>
       <c r="Q4"/>
       <c r="R4"/>
@@ -1230,7 +1243,7 @@
       <c r="Z4"/>
       <c r="AA4"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" s="10"/>
       <c r="B5" s="18" t="s">
         <v>22</v>
@@ -1279,7 +1292,7 @@
       <c r="Z5"/>
       <c r="AA5"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1330,7 +1343,7 @@
       <c r="Z6"/>
       <c r="AA6"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1385,7 +1398,7 @@
       <c r="Z7"/>
       <c r="AA7"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1440,7 +1453,7 @@
       <c r="Z8"/>
       <c r="AA8"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1495,7 +1508,7 @@
       <c r="Z9"/>
       <c r="AA9"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1550,7 +1563,7 @@
       <c r="Z10"/>
       <c r="AA10"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1605,7 +1618,7 @@
       <c r="Z11"/>
       <c r="AA11"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1660,7 +1673,7 @@
       <c r="Z12"/>
       <c r="AA12"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1715,7 +1728,7 @@
       <c r="Z13"/>
       <c r="AA13"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1770,7 +1783,7 @@
       <c r="Z14"/>
       <c r="AA14"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1825,7 +1838,7 @@
       <c r="Z15"/>
       <c r="AA15"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1880,7 +1893,7 @@
       <c r="Z16"/>
       <c r="AA16"/>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1935,7 +1948,7 @@
       <c r="Z17"/>
       <c r="AA17"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1990,7 +2003,7 @@
       <c r="Z18"/>
       <c r="AA18"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2045,7 +2058,7 @@
       <c r="Z19"/>
       <c r="AA19"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -2100,7 +2113,7 @@
       <c r="Z20"/>
       <c r="AA20"/>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -2155,7 +2168,7 @@
       <c r="Z21"/>
       <c r="AA21"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -2210,7 +2223,7 @@
       <c r="Z22"/>
       <c r="AA22"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -2265,7 +2278,7 @@
       <c r="Z23"/>
       <c r="AA23"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2320,44 +2333,44 @@
       <c r="Z24"/>
       <c r="AA24"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A25" s="42" t="s">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A25" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="48" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" s="48" t="s">
-        <v>37</v>
-      </c>
-      <c r="G25" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="H25" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="I25" s="48" t="s">
-        <v>37</v>
-      </c>
-      <c r="J25" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="K25" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="L25" s="48" t="s">
-        <v>37</v>
-      </c>
-      <c r="M25" s="50" t="s">
+      <c r="B25" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="G25" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="I25" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="J25" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="K25" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="L25" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="M25" s="51" t="s">
         <v>37</v>
       </c>
       <c r="N25" s="33"/>
@@ -2375,20 +2388,20 @@
       <c r="Z25"/>
       <c r="AA25"/>
     </row>
-    <row r="26" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="42"/>
-      <c r="B26" s="47"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="49"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="47"/>
-      <c r="L26" s="49"/>
-      <c r="M26" s="51"/>
+    <row r="26" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="43"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="48"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="52"/>
       <c r="N26" s="33"/>
       <c r="O26" s="34"/>
       <c r="P26" s="34"/>
@@ -2400,7 +2413,7 @@
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -2455,7 +2468,7 @@
       <c r="Z27"/>
       <c r="AA27"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>0</v>
       </c>
@@ -2510,7 +2523,7 @@
       <c r="Z28"/>
       <c r="AA28"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
@@ -2528,7 +2541,7 @@
       <c r="Z29"/>
       <c r="AA29"/>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>38</v>
       </c>
@@ -2549,10 +2562,10 @@
       <c r="Z30"/>
       <c r="AA30"/>
     </row>
-    <row r="31" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
@@ -2562,6 +2575,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="M25:M26"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="H4:J4"/>
@@ -2578,11 +2596,6 @@
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="M25:M26"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="78" orientation="landscape" r:id="rId1"/>
@@ -2593,734 +2606,727 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="77.44140625" customWidth="1"/>
+    <col min="1" max="1" width="77.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="43">
+    <row r="2" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N2" s="44"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="54"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" s="17"/>
+      <c r="B3" s="44">
         <v>2017</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="43">
+      <c r="C3" s="45"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="44">
         <v>2018</v>
       </c>
-      <c r="F2" s="52"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="43">
+      <c r="F3" s="45"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="44">
         <v>2019</v>
       </c>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="43">
+      <c r="I3" s="45"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="44">
         <v>2020</v>
       </c>
-      <c r="L2" s="52"/>
-      <c r="M2" s="53"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B3" s="30" t="s">
+      <c r="L3" s="45"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="4"/>
+    </row>
+    <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4"/>
+      <c r="B4" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C4" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E4" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F4" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="H4" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I4" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="30" t="s">
+      <c r="K4" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="L4" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="27" t="s">
+      <c r="M4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-    </row>
-    <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="31">
-        <v>5.307529117073212E-2</v>
-      </c>
-      <c r="C4" s="21">
-        <v>1.2010489223191794E-2</v>
-      </c>
-      <c r="D4" s="25">
-        <v>2.0882259833766462E-2</v>
-      </c>
-      <c r="E4" s="31">
-        <v>4.2254871622770127E-2</v>
-      </c>
-      <c r="F4" s="21">
-        <v>1.0382378742349751E-2</v>
-      </c>
-      <c r="G4" s="25">
-        <v>1.6980440914020505E-2</v>
-      </c>
-      <c r="H4" s="31">
-        <v>5.4093627213741398E-2</v>
-      </c>
-      <c r="I4" s="21">
-        <v>8.2598764725443051E-3</v>
-      </c>
-      <c r="J4" s="25">
-        <v>1.7885965985140678E-2</v>
-      </c>
-      <c r="K4" s="31">
-        <v>4.6239466588826328E-2</v>
-      </c>
-      <c r="L4" s="21">
-        <v>1.1229803259088022E-2</v>
-      </c>
-      <c r="M4" s="25">
-        <v>1.9403806869439048E-2</v>
-      </c>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
       <c r="Q4" s="17"/>
       <c r="R4" s="17"/>
       <c r="S4" s="17"/>
       <c r="T4" s="17"/>
       <c r="U4" s="17"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>24</v>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="B5" s="31">
-        <v>0.12725034292968451</v>
+        <v>5.307529117073212E-2</v>
       </c>
       <c r="C5" s="21">
-        <v>6.4223015722096627E-2</v>
+        <v>1.2010489223191794E-2</v>
       </c>
       <c r="D5" s="25">
-        <v>7.7838227823871967E-2</v>
+        <v>2.0882259833766462E-2</v>
       </c>
       <c r="E5" s="31">
-        <v>0.11069076581779194</v>
+        <v>4.2254871622770127E-2</v>
       </c>
       <c r="F5" s="21">
-        <v>5.6276475065792989E-2</v>
+        <v>1.0382378742349751E-2</v>
       </c>
       <c r="G5" s="25">
-        <v>6.7541012005406312E-2</v>
+        <v>1.6980440914020505E-2</v>
       </c>
       <c r="H5" s="31">
-        <v>0.10218687709685093</v>
+        <v>5.4093627213741398E-2</v>
       </c>
       <c r="I5" s="21">
-        <v>4.5774935810424057E-2</v>
+        <v>8.2598764725443051E-3</v>
       </c>
       <c r="J5" s="25">
-        <v>5.7621647135024143E-2</v>
+        <v>1.7885965985140678E-2</v>
       </c>
       <c r="K5" s="31">
-        <v>6.487121776603344E-2</v>
+        <v>4.6239466588826328E-2</v>
       </c>
       <c r="L5" s="21">
-        <v>4.2502214022571913E-2</v>
+        <v>1.1229803259088022E-2</v>
       </c>
       <c r="M5" s="25">
-        <v>4.7724863739326474E-2</v>
-      </c>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
+        <v>1.9403806869439048E-2</v>
+      </c>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
       <c r="Q5" s="17"/>
       <c r="R5" s="17"/>
       <c r="S5" s="17"/>
       <c r="T5" s="17"/>
       <c r="U5" s="17"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>25</v>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="B6" s="31">
-        <v>1.7670463743173357E-2</v>
+        <v>0.12725034292968451</v>
       </c>
       <c r="C6" s="21">
-        <v>6.3292179330971619E-3</v>
+        <v>6.4223015722096627E-2</v>
       </c>
       <c r="D6" s="25">
-        <v>8.7791626482518967E-3</v>
+        <v>7.7838227823871967E-2</v>
       </c>
       <c r="E6" s="31">
-        <v>9.5710879921199789E-3</v>
+        <v>0.11069076581779194</v>
       </c>
       <c r="F6" s="21">
-        <v>7.2295489894674322E-3</v>
+        <v>5.6276475065792989E-2</v>
       </c>
       <c r="G6" s="25">
-        <v>7.7142810741166468E-3</v>
+        <v>6.7541012005406312E-2</v>
       </c>
       <c r="H6" s="31">
-        <v>9.7818864891025276E-3</v>
+        <v>0.10218687709685093</v>
       </c>
       <c r="I6" s="21">
-        <v>4.4123178569676355E-3</v>
+        <v>4.5774935810424057E-2</v>
       </c>
       <c r="J6" s="25">
-        <v>5.5399467021296752E-3</v>
+        <v>5.7621647135024143E-2</v>
       </c>
       <c r="K6" s="31">
-        <v>1.884683632788195E-2</v>
+        <v>6.487121776603344E-2</v>
       </c>
       <c r="L6" s="21">
-        <v>6.9105581676667301E-3</v>
+        <v>4.2502214022571913E-2</v>
       </c>
       <c r="M6" s="25">
-        <v>9.6974197008094041E-3</v>
-      </c>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
+        <v>4.7724863739326474E-2</v>
+      </c>
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="41"/>
       <c r="Q6" s="17"/>
       <c r="R6" s="17"/>
       <c r="S6" s="39"/>
       <c r="T6" s="39"/>
       <c r="U6" s="39"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>26</v>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="B7" s="31">
-        <v>5.5375689054366073E-2</v>
+        <v>1.7670463743173357E-2</v>
       </c>
       <c r="C7" s="21">
-        <v>2.8995612274363147E-2</v>
+        <v>6.3292179330971619E-3</v>
       </c>
       <c r="D7" s="25">
-        <v>3.4694256918421887E-2</v>
+        <v>8.7791626482518967E-3</v>
       </c>
       <c r="E7" s="31">
-        <v>4.9716484847956557E-2</v>
+        <v>9.5710879921199789E-3</v>
       </c>
       <c r="F7" s="21">
-        <v>3.9299436905288809E-2</v>
+        <v>7.2295489894674322E-3</v>
       </c>
       <c r="G7" s="25">
-        <v>4.1455914913735389E-2</v>
+        <v>7.7142810741166468E-3</v>
       </c>
       <c r="H7" s="31">
-        <v>5.6870288493876583E-2</v>
+        <v>9.7818864891025276E-3</v>
       </c>
       <c r="I7" s="21">
-        <v>3.3580279217841159E-2</v>
+        <v>4.4123178569676355E-3</v>
       </c>
       <c r="J7" s="25">
-        <v>3.8471277891375014E-2</v>
+        <v>5.5399467021296752E-3</v>
       </c>
       <c r="K7" s="31">
-        <v>6.627311205168189E-2</v>
+        <v>1.884683632788195E-2</v>
       </c>
       <c r="L7" s="21">
-        <v>3.2072617600572777E-2</v>
+        <v>6.9105581676667301E-3</v>
       </c>
       <c r="M7" s="25">
-        <v>4.0057678753019792E-2</v>
-      </c>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
+        <v>9.6974197008094041E-3</v>
+      </c>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="41"/>
       <c r="Q7" s="17"/>
       <c r="R7" s="17"/>
       <c r="S7" s="39"/>
       <c r="T7" s="39"/>
       <c r="U7" s="39"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>27</v>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="B8" s="31">
-        <v>8.3534263148477908E-2</v>
+        <v>5.5375689054366073E-2</v>
       </c>
       <c r="C8" s="21">
-        <v>3.085376360746641E-2</v>
+        <v>2.8995612274363147E-2</v>
       </c>
       <c r="D8" s="25">
-        <v>4.2233845972628151E-2</v>
+        <v>3.4694256918421887E-2</v>
       </c>
       <c r="E8" s="31">
-        <v>8.0168757981354685E-2</v>
+        <v>4.9716484847956557E-2</v>
       </c>
       <c r="F8" s="21">
-        <v>3.2841312878814602E-2</v>
+        <v>3.9299436905288809E-2</v>
       </c>
       <c r="G8" s="25">
-        <v>4.2638771345099941E-2</v>
+        <v>4.1455914913735389E-2</v>
       </c>
       <c r="H8" s="31">
-        <v>8.9123854678489697E-2</v>
+        <v>5.6870288493876583E-2</v>
       </c>
       <c r="I8" s="21">
-        <v>3.8678376153640677E-2</v>
+        <v>3.3580279217841159E-2</v>
       </c>
       <c r="J8" s="25">
-        <v>4.927210681623604E-2</v>
+        <v>3.8471277891375014E-2</v>
       </c>
       <c r="K8" s="31">
-        <v>8.8530584340264715E-2</v>
+        <v>6.627311205168189E-2</v>
       </c>
       <c r="L8" s="21">
-        <v>4.7315153975472021E-2</v>
+        <v>3.2072617600572777E-2</v>
       </c>
       <c r="M8" s="25">
-        <v>5.6938040177842819E-2</v>
-      </c>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
+        <v>4.0057678753019792E-2</v>
+      </c>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="41"/>
       <c r="Q8" s="17"/>
       <c r="R8" s="17"/>
       <c r="S8" s="39"/>
       <c r="T8" s="39"/>
       <c r="U8" s="39"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>28</v>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="B9" s="31">
-        <v>7.1154714537662631E-2</v>
+        <v>8.3534263148477908E-2</v>
       </c>
       <c r="C9" s="21">
-        <v>6.1024366080462765E-2</v>
+        <v>3.085376360746641E-2</v>
       </c>
       <c r="D9" s="25">
-        <v>6.3213652058041858E-2</v>
+        <v>4.2233845972628151E-2</v>
       </c>
       <c r="E9" s="31">
-        <v>8.0465130469270965E-2</v>
+        <v>8.0168757981354685E-2</v>
       </c>
       <c r="F9" s="21">
-        <v>7.0982474544682914E-2</v>
+        <v>3.2841312878814602E-2</v>
       </c>
       <c r="G9" s="25">
-        <v>7.2945520032769912E-2</v>
+        <v>4.2638771345099941E-2</v>
       </c>
       <c r="H9" s="31">
-        <v>8.8996710661230924E-2</v>
+        <v>8.9123854678489697E-2</v>
       </c>
       <c r="I9" s="21">
-        <v>6.7741671709159887E-2</v>
+        <v>3.8678376153640677E-2</v>
       </c>
       <c r="J9" s="25">
-        <v>7.2205350113951336E-2</v>
+        <v>4.927210681623604E-2</v>
       </c>
       <c r="K9" s="31">
-        <v>9.9676604112735351E-2</v>
+        <v>8.8530584340264715E-2</v>
       </c>
       <c r="L9" s="21">
-        <v>7.522061257939186E-2</v>
+        <v>4.7315153975472021E-2</v>
       </c>
       <c r="M9" s="25">
-        <v>8.093050033089956E-2</v>
-      </c>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
+        <v>5.6938040177842819E-2</v>
+      </c>
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
       <c r="Q9" s="17"/>
       <c r="R9" s="17"/>
       <c r="S9" s="39"/>
       <c r="T9" s="39"/>
       <c r="U9" s="39"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>29</v>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="B10" s="31">
-        <v>1.0232510586090262E-2</v>
+        <v>7.1154714537662631E-2</v>
       </c>
       <c r="C10" s="21">
-        <v>6.9102570423113857E-3</v>
+        <v>6.1024366080462765E-2</v>
       </c>
       <c r="D10" s="25">
-        <v>7.6270125816259669E-3</v>
+        <v>6.3213652058041858E-2</v>
       </c>
       <c r="E10" s="31">
-        <v>6.0407686507642491E-3</v>
+        <v>8.0465130469270965E-2</v>
       </c>
       <c r="F10" s="21">
-        <v>6.8438365079708224E-3</v>
+        <v>7.0982474544682914E-2</v>
       </c>
       <c r="G10" s="25">
-        <v>6.6775899683669364E-3</v>
+        <v>7.2945520032769912E-2</v>
       </c>
       <c r="H10" s="31">
-        <v>2.1503744596379267E-2</v>
+        <v>8.8996710661230924E-2</v>
       </c>
       <c r="I10" s="21">
-        <v>7.9044488418619618E-3</v>
+        <v>6.7741671709159887E-2</v>
       </c>
       <c r="J10" s="25">
-        <v>1.0760347349145839E-2</v>
+        <v>7.2205350113951336E-2</v>
       </c>
       <c r="K10" s="31">
-        <v>1.0969342684416314E-2</v>
+        <v>9.9676604112735351E-2</v>
       </c>
       <c r="L10" s="21">
-        <v>8.0161070873290049E-3</v>
+        <v>7.522061257939186E-2</v>
       </c>
       <c r="M10" s="25">
-        <v>8.7056177598906683E-3</v>
-      </c>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
+        <v>8.093050033089956E-2</v>
+      </c>
+      <c r="N10" s="41"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
       <c r="Q10" s="17"/>
       <c r="R10" s="17"/>
       <c r="S10" s="39"/>
       <c r="T10" s="39"/>
       <c r="U10" s="39"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>30</v>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="B11" s="31">
-        <v>6.1727343210844249E-2</v>
+        <v>1.0232510586090262E-2</v>
       </c>
       <c r="C11" s="21">
-        <v>0.24625728646519282</v>
+        <v>6.9102570423113857E-3</v>
       </c>
       <c r="D11" s="25">
-        <v>0.20639498501836814</v>
+        <v>7.6270125816259669E-3</v>
       </c>
       <c r="E11" s="31">
-        <v>7.8625877676614025E-2</v>
+        <v>6.0407686507642491E-3</v>
       </c>
       <c r="F11" s="21">
-        <v>0.24938189290391435</v>
+        <v>6.8438365079708224E-3</v>
       </c>
       <c r="G11" s="25">
-        <v>0.21403295396514047</v>
+        <v>6.6775899683669364E-3</v>
       </c>
       <c r="H11" s="31">
-        <v>7.5683501628263705E-2</v>
+        <v>2.1503744596379267E-2</v>
       </c>
       <c r="I11" s="21">
-        <v>0.25040312689093497</v>
+        <v>7.9044488418619618E-3</v>
       </c>
       <c r="J11" s="25">
-        <v>0.21371171261181959</v>
+        <v>1.0760347349145839E-2</v>
       </c>
       <c r="K11" s="31">
-        <v>7.5782948356518998E-2</v>
+        <v>1.0969342684416314E-2</v>
       </c>
       <c r="L11" s="21">
-        <v>0.24028199101756126</v>
+        <v>8.0161070873290049E-3</v>
       </c>
       <c r="M11" s="25">
-        <v>0.20187473882249973</v>
-      </c>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
+        <v>8.7056177598906683E-3</v>
+      </c>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
       <c r="Q11" s="17"/>
       <c r="R11" s="17"/>
       <c r="S11" s="39"/>
       <c r="T11" s="39"/>
       <c r="U11" s="39"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>31</v>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="B12" s="31">
-        <v>0.21840573906672006</v>
+        <v>6.1727343210844249E-2</v>
       </c>
       <c r="C12" s="21">
-        <v>0.25336004939419338</v>
+        <v>0.24625728646519282</v>
       </c>
       <c r="D12" s="25">
-        <v>0.24580919216979674</v>
+        <v>0.20639498501836814</v>
       </c>
       <c r="E12" s="31">
-        <v>0.19770224153486082</v>
+        <v>7.8625877676614025E-2</v>
       </c>
       <c r="F12" s="21">
-        <v>0.20398273737531189</v>
+        <v>0.24938189290391435</v>
       </c>
       <c r="G12" s="25">
-        <v>0.20268258485258053</v>
+        <v>0.21403295396514047</v>
       </c>
       <c r="H12" s="31">
-        <v>0.1325045730832014</v>
+        <v>7.5683501628263705E-2</v>
       </c>
       <c r="I12" s="21">
-        <v>0.20171826363789994</v>
+        <v>0.25040312689093497</v>
       </c>
       <c r="J12" s="25">
-        <v>0.1871842221766685</v>
+        <v>0.21371171261181959</v>
       </c>
       <c r="K12" s="31">
-        <v>0.11270077814734869</v>
+        <v>7.5782948356518998E-2</v>
       </c>
       <c r="L12" s="21">
-        <v>0.20222069096222534</v>
+        <v>0.24028199101756126</v>
       </c>
       <c r="M12" s="25">
-        <v>0.18131950908494165</v>
-      </c>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
+        <v>0.20187473882249973</v>
+      </c>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
       <c r="Q12" s="17"/>
       <c r="R12" s="17"/>
       <c r="S12" s="39"/>
       <c r="T12" s="39"/>
       <c r="U12" s="39"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>32</v>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="B13" s="31">
-        <v>7.3016332824973801E-2</v>
+        <v>0.21840573906672006</v>
       </c>
       <c r="C13" s="21">
-        <v>8.1992248116611613E-2</v>
+        <v>0.25336004939419338</v>
       </c>
       <c r="D13" s="25">
-        <v>8.0053263934390023E-2</v>
+        <v>0.24580919216979674</v>
       </c>
       <c r="E13" s="31">
-        <v>6.5493961410558701E-2</v>
+        <v>0.19770224153486082</v>
       </c>
       <c r="F13" s="21">
-        <v>9.6116364563149329E-2</v>
+        <v>0.20398273737531189</v>
       </c>
       <c r="G13" s="25">
-        <v>8.9776186600790009E-2</v>
+        <v>0.20268258485258053</v>
       </c>
       <c r="H13" s="31">
-        <v>7.5556357611004932E-2</v>
+        <v>0.1325045730832014</v>
       </c>
       <c r="I13" s="21">
-        <v>0.10349921773213186</v>
+        <v>0.20171826363789994</v>
       </c>
       <c r="J13" s="25">
-        <v>9.7631224903576327E-2</v>
+        <v>0.1871842221766685</v>
       </c>
       <c r="K13" s="31">
-        <v>6.4659973421620665E-2</v>
+        <v>0.11270077814734869</v>
       </c>
       <c r="L13" s="21">
-        <v>9.4198617420409247E-2</v>
+        <v>0.20222069096222534</v>
       </c>
       <c r="M13" s="25">
-        <v>8.730188621718131E-2</v>
-      </c>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
+        <v>0.18131950908494165</v>
+      </c>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
       <c r="Q13" s="17"/>
       <c r="R13" s="17"/>
       <c r="S13" s="39"/>
       <c r="T13" s="39"/>
       <c r="U13" s="39"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>33</v>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="B14" s="31">
-        <v>0.161858551090133</v>
+        <v>7.3016332824973801E-2</v>
       </c>
       <c r="C14" s="21">
-        <v>0.16668075246325367</v>
+        <v>8.1992248116611613E-2</v>
       </c>
       <c r="D14" s="25">
-        <v>0.16563905678296142</v>
+        <v>8.0053263934390023E-2</v>
       </c>
       <c r="E14" s="31">
-        <v>0.16516228572922886</v>
+        <v>6.5493961410558701E-2</v>
       </c>
       <c r="F14" s="21">
-        <v>0.16499391848609557</v>
+        <v>9.6116364563149329E-2</v>
       </c>
       <c r="G14" s="25">
-        <v>0.16502787065992741</v>
+        <v>8.9776186600790009E-2</v>
       </c>
       <c r="H14" s="31">
-        <v>0.17570893043171545</v>
+        <v>7.5556357611004932E-2</v>
       </c>
       <c r="I14" s="21">
-        <v>0.17799292415545054</v>
+        <v>0.10349921773213186</v>
       </c>
       <c r="J14" s="25">
-        <v>0.17751429344146794</v>
+        <v>9.7631224903576327E-2</v>
       </c>
       <c r="K14" s="31">
-        <v>0.2101996451095014</v>
+        <v>6.4659973421620665E-2</v>
       </c>
       <c r="L14" s="21">
-        <v>0.17161979880179556</v>
+        <v>9.4198617420409247E-2</v>
       </c>
       <c r="M14" s="25">
-        <v>0.18062722056921898</v>
-      </c>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
+        <v>8.730188621718131E-2</v>
+      </c>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
       <c r="Q14" s="17"/>
       <c r="R14" s="17"/>
       <c r="S14" s="39"/>
       <c r="T14" s="39"/>
       <c r="U14" s="39"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>34</v>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="B15" s="31">
-        <v>6.6703018633222852E-2</v>
+        <v>0.161858551090133</v>
       </c>
       <c r="C15" s="21">
-        <v>4.1362941677759231E-2</v>
+        <v>0.16668075246325367</v>
       </c>
       <c r="D15" s="25">
-        <v>4.6836924753189575E-2</v>
+        <v>0.16563905678296142</v>
       </c>
       <c r="E15" s="31">
-        <v>0.11411212468564903</v>
+        <v>0.16516228572922886</v>
       </c>
       <c r="F15" s="21">
-        <v>6.1670760832092192E-2</v>
+        <v>0.16499391848609557</v>
       </c>
       <c r="G15" s="25">
-        <v>7.2526873668045916E-2</v>
+        <v>0.16502787065992741</v>
       </c>
       <c r="H15" s="31">
-        <v>0.11798144517632005</v>
+        <v>0.17570893043171545</v>
       </c>
       <c r="I15" s="21">
-        <v>6.0033471252337267E-2</v>
+        <v>0.17799292415545054</v>
       </c>
       <c r="J15" s="25">
-        <v>7.2202766183586536E-2</v>
+        <v>0.17751429344146794</v>
       </c>
       <c r="K15" s="31">
-        <v>0.14125333189943232</v>
+        <v>0.2101996451095014</v>
       </c>
       <c r="L15" s="21">
-        <v>6.8413004998952948E-2</v>
+        <v>0.17161979880179556</v>
       </c>
       <c r="M15" s="25">
-        <v>8.541961472171257E-2</v>
-      </c>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
+        <v>0.18062722056921898</v>
+      </c>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
       <c r="Q15" s="17"/>
       <c r="R15" s="17"/>
       <c r="S15" s="39"/>
       <c r="T15" s="39"/>
       <c r="U15" s="39"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="32">
-        <v>1</v>
-      </c>
-      <c r="C16" s="28">
-        <v>1</v>
-      </c>
-      <c r="D16" s="29">
-        <v>1</v>
-      </c>
-      <c r="E16" s="32">
-        <v>1</v>
-      </c>
-      <c r="F16" s="28">
-        <v>1</v>
-      </c>
-      <c r="G16" s="29">
-        <v>1</v>
-      </c>
-      <c r="H16" s="32">
-        <v>1</v>
-      </c>
-      <c r="I16" s="28">
-        <v>1</v>
-      </c>
-      <c r="J16" s="29">
-        <v>1</v>
-      </c>
-      <c r="K16" s="32">
-        <v>1</v>
-      </c>
-      <c r="L16" s="28">
-        <v>1</v>
-      </c>
-      <c r="M16" s="29">
-        <v>1</v>
-      </c>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="31">
+        <v>6.6703018633222852E-2</v>
+      </c>
+      <c r="C16" s="21">
+        <v>4.1362941677759231E-2</v>
+      </c>
+      <c r="D16" s="25">
+        <v>4.6836924753189575E-2</v>
+      </c>
+      <c r="E16" s="31">
+        <v>0.11411212468564903</v>
+      </c>
+      <c r="F16" s="21">
+        <v>6.1670760832092192E-2</v>
+      </c>
+      <c r="G16" s="25">
+        <v>7.2526873668045916E-2</v>
+      </c>
+      <c r="H16" s="31">
+        <v>0.11798144517632005</v>
+      </c>
+      <c r="I16" s="21">
+        <v>6.0033471252337267E-2</v>
+      </c>
+      <c r="J16" s="25">
+        <v>7.2202766183586536E-2</v>
+      </c>
+      <c r="K16" s="31">
+        <v>0.14125333189943232</v>
+      </c>
+      <c r="L16" s="21">
+        <v>6.8413004998952948E-2</v>
+      </c>
+      <c r="M16" s="25">
+        <v>8.541961472171257E-2</v>
+      </c>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="41"/>
       <c r="Q16" s="17"/>
       <c r="R16" s="17"/>
       <c r="S16" s="39"/>
       <c r="T16" s="39"/>
       <c r="U16" s="39"/>
     </row>
-    <row r="17" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
+    <row r="17" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="28">
+        <v>1</v>
+      </c>
+      <c r="C17" s="28">
+        <v>1</v>
+      </c>
+      <c r="D17" s="29">
+        <v>1</v>
+      </c>
+      <c r="E17" s="32">
+        <v>1</v>
+      </c>
+      <c r="F17" s="28">
+        <v>1</v>
+      </c>
+      <c r="G17" s="29">
+        <v>1</v>
+      </c>
+      <c r="H17" s="32">
+        <v>1</v>
+      </c>
+      <c r="I17" s="28">
+        <v>1</v>
+      </c>
+      <c r="J17" s="29">
+        <v>1</v>
+      </c>
+      <c r="K17" s="32">
+        <v>1</v>
+      </c>
+      <c r="L17" s="28">
+        <v>1</v>
+      </c>
+      <c r="M17" s="29">
+        <v>1</v>
+      </c>
       <c r="N17" s="17"/>
       <c r="O17" s="17"/>
       <c r="P17" s="17"/>
@@ -3330,7 +3336,7 @@
       <c r="T17" s="39"/>
       <c r="U17" s="39"/>
     </row>
-    <row r="18" spans="1:21" s="4" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" s="4" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -3346,7 +3352,7 @@
       <c r="T18" s="39"/>
       <c r="U18" s="39"/>
     </row>
-    <row r="19" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -3362,7 +3368,7 @@
       <c r="T19" s="17"/>
       <c r="U19" s="17"/>
     </row>
-    <row r="20" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -3378,7 +3384,7 @@
       <c r="T20" s="17"/>
       <c r="U20" s="17"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -3387,34 +3393,34 @@
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="24" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3423,7 +3429,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3432,7 +3438,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -3441,7 +3447,7 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" s="4"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -3450,7 +3456,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3459,7 +3465,7 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="4"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -3468,7 +3474,7 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="4"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -3477,105 +3483,105 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
     </row>
-    <row r="44" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
     </row>
-    <row r="46" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
     </row>
-    <row r="47" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
     </row>
-    <row r="48" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="2:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -3583,13 +3589,480 @@
       <c r="M49" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
+  <mergeCells count="5">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA9708F-A427-42FB-9C29-BF04FE0ACBE8}">
+  <dimension ref="D8:H41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="72.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D8" s="17"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="57"/>
+    </row>
+    <row r="9" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="55">
+        <v>2017</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="21">
+        <v>1.2010489223191794E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="55">
+        <v>2017</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="31">
+        <v>5.307529117073212E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="55">
+        <v>2017</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="25">
+        <v>2.0882259833766462E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="55">
+        <v>2017</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="55">
+        <v>2017</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D15" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="55">
+        <v>2017</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="31">
+        <v>0.12725034292968451</v>
+      </c>
+      <c r="G18" s="21">
+        <v>6.4223015722096627E-2</v>
+      </c>
+      <c r="H18" s="25">
+        <v>7.7838227823871967E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="31">
+        <v>1.7670463743173357E-2</v>
+      </c>
+      <c r="G19" s="21">
+        <v>6.3292179330971619E-3</v>
+      </c>
+      <c r="H19" s="25">
+        <v>8.7791626482518967E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="31">
+        <v>5.5375689054366073E-2</v>
+      </c>
+      <c r="G20" s="21">
+        <v>2.8995612274363147E-2</v>
+      </c>
+      <c r="H20" s="25">
+        <v>3.4694256918421887E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="31">
+        <v>8.3534263148477908E-2</v>
+      </c>
+      <c r="G21" s="21">
+        <v>3.085376360746641E-2</v>
+      </c>
+      <c r="H21" s="25">
+        <v>4.2233845972628151E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="31">
+        <v>7.1154714537662631E-2</v>
+      </c>
+      <c r="G22" s="21">
+        <v>6.1024366080462765E-2</v>
+      </c>
+      <c r="H22" s="25">
+        <v>6.3213652058041858E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="31">
+        <v>1.0232510586090262E-2</v>
+      </c>
+      <c r="G23" s="21">
+        <v>6.9102570423113857E-3</v>
+      </c>
+      <c r="H23" s="25">
+        <v>7.6270125816259669E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D24" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="31">
+        <v>6.1727343210844249E-2</v>
+      </c>
+      <c r="G24" s="21">
+        <v>0.24625728646519282</v>
+      </c>
+      <c r="H24" s="25">
+        <v>0.20639498501836814</v>
+      </c>
+    </row>
+    <row r="25" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D25" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="31">
+        <v>0.21840573906672006</v>
+      </c>
+      <c r="G25" s="21">
+        <v>0.25336004939419338</v>
+      </c>
+      <c r="H25" s="25">
+        <v>0.24580919216979674</v>
+      </c>
+    </row>
+    <row r="26" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D26" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="31">
+        <v>7.3016332824973801E-2</v>
+      </c>
+      <c r="G26" s="21">
+        <v>8.1992248116611613E-2</v>
+      </c>
+      <c r="H26" s="25">
+        <v>8.0053263934390023E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D27" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="31">
+        <v>0.161858551090133</v>
+      </c>
+      <c r="G27" s="21">
+        <v>0.16668075246325367</v>
+      </c>
+      <c r="H27" s="25">
+        <v>0.16563905678296142</v>
+      </c>
+    </row>
+    <row r="28" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="31">
+        <v>6.6703018633222852E-2</v>
+      </c>
+      <c r="G28" s="21">
+        <v>4.1362941677759231E-2</v>
+      </c>
+      <c r="H28" s="25">
+        <v>4.6836924753189575E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="F29" s="58">
+        <v>1</v>
+      </c>
+      <c r="G29" s="28">
+        <v>1</v>
+      </c>
+      <c r="H29" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D30" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="31">
+        <v>0.12725034292968451</v>
+      </c>
+      <c r="G30" s="21">
+        <v>6.4223015722096627E-2</v>
+      </c>
+      <c r="H30" s="25">
+        <v>7.7838227823871967E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="31">
+        <v>1.7670463743173357E-2</v>
+      </c>
+      <c r="G31" s="21">
+        <v>6.3292179330971619E-3</v>
+      </c>
+      <c r="H31" s="25">
+        <v>8.7791626482518967E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="31">
+        <v>5.5375689054366073E-2</v>
+      </c>
+      <c r="G32" s="21">
+        <v>2.8995612274363147E-2</v>
+      </c>
+      <c r="H32" s="25">
+        <v>3.4694256918421887E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D33" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="31">
+        <v>8.3534263148477908E-2</v>
+      </c>
+      <c r="G33" s="21">
+        <v>3.085376360746641E-2</v>
+      </c>
+      <c r="H33" s="25">
+        <v>4.2233845972628151E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" s="31">
+        <v>7.1154714537662631E-2</v>
+      </c>
+      <c r="G34" s="21">
+        <v>6.1024366080462765E-2</v>
+      </c>
+      <c r="H34" s="25">
+        <v>6.3213652058041858E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D35" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="31">
+        <v>1.0232510586090262E-2</v>
+      </c>
+      <c r="G35" s="21">
+        <v>6.9102570423113857E-3</v>
+      </c>
+      <c r="H35" s="25">
+        <v>7.6270125816259669E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D36" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="31">
+        <v>6.1727343210844249E-2</v>
+      </c>
+      <c r="G36" s="21">
+        <v>0.24625728646519282</v>
+      </c>
+      <c r="H36" s="25">
+        <v>0.20639498501836814</v>
+      </c>
+    </row>
+    <row r="37" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D37" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="31">
+        <v>0.21840573906672006</v>
+      </c>
+      <c r="G37" s="21">
+        <v>0.25336004939419338</v>
+      </c>
+      <c r="H37" s="25">
+        <v>0.24580919216979674</v>
+      </c>
+    </row>
+    <row r="38" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D38" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="31">
+        <v>7.3016332824973801E-2</v>
+      </c>
+      <c r="G38" s="21">
+        <v>8.1992248116611613E-2</v>
+      </c>
+      <c r="H38" s="25">
+        <v>8.0053263934390023E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D39" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="31">
+        <v>0.161858551090133</v>
+      </c>
+      <c r="G39" s="21">
+        <v>0.16668075246325367</v>
+      </c>
+      <c r="H39" s="25">
+        <v>0.16563905678296142</v>
+      </c>
+    </row>
+    <row r="40" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D40" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="31">
+        <v>6.6703018633222852E-2</v>
+      </c>
+      <c r="G40" s="21">
+        <v>4.1362941677759231E-2</v>
+      </c>
+      <c r="H40" s="25">
+        <v>4.6836924753189575E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="58">
+        <v>1</v>
+      </c>
+      <c r="G41" s="28">
+        <v>1</v>
+      </c>
+      <c r="H41" s="29">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F31823-6639-43B9-8826-B51812B8CA5A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>